<commit_message>
data handeling for tests
</commit_message>
<xml_diff>
--- a/test/test_daten.xlsx
+++ b/test/test_daten.xlsx
@@ -33,7 +33,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +44,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -77,16 +83,16 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -423,7 +429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>1.5</v>
       </c>
@@ -437,7 +443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>2.5</v>
       </c>
@@ -451,7 +457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>3.5</v>
       </c>
@@ -465,7 +471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>4.5</v>
       </c>
@@ -479,7 +485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>5.5</v>
       </c>

</xml_diff>